<commit_message>
mod by zkj @20171202
</commit_message>
<xml_diff>
--- a/xboost/com.xboost.business/src/main/webapp/static/excelTemplate/distances.xlsx
+++ b/xboost/com.xboost.business/src/main/webapp/static/excelTemplate/distances.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8370"/>
+    <workbookView windowWidth="20580" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6">
   <si>
     <t>from</t>
   </si>
@@ -35,30 +35,6 @@
   <si>
     <t>571AD</t>
   </si>
-  <si>
-    <t>571AF</t>
-  </si>
-  <si>
-    <t>571AG</t>
-  </si>
-  <si>
-    <t>571AC</t>
-  </si>
-  <si>
-    <t>571AQ</t>
-  </si>
-  <si>
-    <t>571AM</t>
-  </si>
-  <si>
-    <t>571AB</t>
-  </si>
-  <si>
-    <t>571JC</t>
-  </si>
-  <si>
-    <t>571KH</t>
-  </si>
 </sst>
 </file>
 
@@ -66,9 +42,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -80,6 +56,43 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -87,60 +100,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -154,23 +128,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -178,14 +138,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -208,8 +160,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -218,6 +171,29 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -232,37 +208,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -274,31 +346,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -310,109 +382,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -423,15 +399,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -446,6 +413,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -499,16 +475,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -523,6 +490,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -531,10 +507,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -543,133 +519,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1031,7 +1007,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
@@ -1061,123 +1037,59 @@
         <v>5</v>
       </c>
       <c r="C2" s="1">
-        <v>10.119</v>
+        <v>120.119</v>
       </c>
       <c r="D2" s="1">
-        <v>20.238</v>
+        <v>120.238</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1">
-        <v>6.543</v>
-      </c>
-      <c r="D3" s="1">
-        <v>13.086</v>
-      </c>
+      <c r="A3"/>
+      <c r="B3"/>
+      <c r="C3"/>
+      <c r="D3"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1">
-        <v>19.269</v>
-      </c>
-      <c r="D4" s="1">
-        <v>38.538</v>
-      </c>
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1">
-        <v>27.293</v>
-      </c>
-      <c r="D5" s="1">
-        <v>54.586</v>
-      </c>
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1">
-        <v>36.776</v>
-      </c>
-      <c r="D6" s="1">
-        <v>73.552</v>
-      </c>
+      <c r="A6"/>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="1">
-        <v>8.363</v>
-      </c>
-      <c r="D7" s="1">
-        <v>16.726</v>
-      </c>
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="1">
-        <v>49.323</v>
-      </c>
-      <c r="D8" s="1">
-        <v>98.646</v>
-      </c>
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="1">
-        <v>50.545</v>
-      </c>
-      <c r="D9" s="1">
-        <v>101.09</v>
-      </c>
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="1">
-        <v>60.06</v>
-      </c>
-      <c r="D10" s="1">
-        <v>120.12</v>
-      </c>
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
     </row>
   </sheetData>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>